<commit_message>
Update tools & config
</commit_message>
<xml_diff>
--- a/Special Challenge/SpcecialChallengeconfig.xlsx
+++ b/Special Challenge/SpcecialChallengeconfig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fotoable/Gamedev_Tools/Special Challenge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{878653AF-83D2-7C4A-A6BB-E87BC9BA0FEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB6C1FB2-8F04-104E-B302-16A06CE69604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2500" yWindow="-21100" windowWidth="35900" windowHeight="21100" xr2:uid="{862DBE92-8EE1-7F40-88FE-3AD3F4281EF4}"/>
+    <workbookView xWindow="-1420" yWindow="-21100" windowWidth="35900" windowHeight="21100" xr2:uid="{862DBE92-8EE1-7F40-88FE-3AD3F4281EF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -462,10 +462,10 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -782,8 +782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E49281F-4F69-0A4E-BEBA-98DF452F93F8}">
   <dimension ref="A1:AD140"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="101" workbookViewId="0">
+      <selection activeCell="G84" sqref="G84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -909,7 +909,7 @@
       <c r="A5" t="s">
         <v>92</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <v>44423.625</v>
       </c>
     </row>
@@ -917,7 +917,7 @@
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="9">
         <v>44427.625</v>
       </c>
     </row>
@@ -1327,12 +1327,12 @@
       </c>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="9" t="s">
+      <c r="A61" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B61" s="9"/>
-      <c r="C61" s="9"/>
-      <c r="D61" s="9"/>
+      <c r="B61" s="10"/>
+      <c r="C61" s="10"/>
+      <c r="D61" s="10"/>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
@@ -1515,12 +1515,12 @@
       </c>
     </row>
     <row r="85" spans="1:4">
-      <c r="A85" s="9" t="s">
+      <c r="A85" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B85" s="9"/>
-      <c r="C85" s="9"/>
-      <c r="D85" s="9"/>
+      <c r="B85" s="10"/>
+      <c r="C85" s="10"/>
+      <c r="D85" s="10"/>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" t="s">
@@ -1621,10 +1621,10 @@
       </c>
     </row>
     <row r="99" spans="1:16">
-      <c r="A99" s="9" t="s">
+      <c r="A99" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="B99" s="9"/>
+      <c r="B99" s="10"/>
     </row>
     <row r="100" spans="1:16">
       <c r="A100" t="s">
@@ -1656,24 +1656,24 @@
       </c>
     </row>
     <row r="106" spans="1:16">
-      <c r="A106" s="9" t="s">
+      <c r="A106" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="B106" s="9"/>
-      <c r="C106" s="9"/>
-      <c r="D106" s="9"/>
-      <c r="E106" s="9"/>
-      <c r="F106" s="9"/>
-      <c r="G106" s="9"/>
-      <c r="H106" s="9"/>
-      <c r="I106" s="9"/>
-      <c r="J106" s="9"/>
-      <c r="K106" s="9"/>
-      <c r="L106" s="9"/>
-      <c r="M106" s="9"/>
-      <c r="N106" s="9"/>
-      <c r="O106" s="9"/>
-      <c r="P106" s="9"/>
+      <c r="B106" s="10"/>
+      <c r="C106" s="10"/>
+      <c r="D106" s="10"/>
+      <c r="E106" s="10"/>
+      <c r="F106" s="10"/>
+      <c r="G106" s="10"/>
+      <c r="H106" s="10"/>
+      <c r="I106" s="10"/>
+      <c r="J106" s="10"/>
+      <c r="K106" s="10"/>
+      <c r="L106" s="10"/>
+      <c r="M106" s="10"/>
+      <c r="N106" s="10"/>
+      <c r="O106" s="10"/>
+      <c r="P106" s="10"/>
     </row>
     <row r="107" spans="1:16">
       <c r="B107" t="s">
@@ -1688,20 +1688,20 @@
       <c r="F107" t="s">
         <v>120</v>
       </c>
-      <c r="G107" s="9" t="s">
+      <c r="G107" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="H107" s="9"/>
-      <c r="I107" s="9"/>
-      <c r="J107" s="9"/>
-      <c r="K107" s="9"/>
-      <c r="L107" s="9" t="s">
+      <c r="H107" s="10"/>
+      <c r="I107" s="10"/>
+      <c r="J107" s="10"/>
+      <c r="K107" s="10"/>
+      <c r="L107" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="M107" s="9"/>
-      <c r="N107" s="9"/>
-      <c r="O107" s="9"/>
-      <c r="P107" s="9"/>
+      <c r="M107" s="10"/>
+      <c r="N107" s="10"/>
+      <c r="O107" s="10"/>
+      <c r="P107" s="10"/>
     </row>
     <row r="108" spans="1:16">
       <c r="A108" t="s">
@@ -2575,10 +2575,10 @@
       </c>
     </row>
     <row r="134" spans="1:16">
-      <c r="A134" s="9" t="s">
+      <c r="A134" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="B134" s="9"/>
+      <c r="B134" s="10"/>
     </row>
     <row r="135" spans="1:16" s="3" customFormat="1">
       <c r="A135" s="4" t="s">

</xml_diff>